<commit_message>
#Added: TDF/3TC/DTG Drug replaces Efavirenz 400mg in CDRR
</commit_message>
<xml_diff>
--- a/assets/templates/orders/v2/cdrr_aggregate.xlsx
+++ b/assets/templates/orders/v2/cdrr_aggregate.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18528"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -452,9 +452,6 @@
     <t>Darunavir (DRV) 600mg tabs</t>
   </si>
   <si>
-    <t>Efavirenz (EFV) 400mg tabs</t>
-  </si>
-  <si>
     <t>Etravirine (ETV) 200mg tabs</t>
   </si>
   <si>
@@ -543,6 +540,9 @@
   </si>
   <si>
     <t>Isoniazid (H) 300mg Tabs</t>
+  </si>
+  <si>
+    <t>Tenofovir/Lamivudine/Dolutegravir (TDF/3TC/DTG) FDC (300/300/50mg) Tabs</t>
   </si>
 </sst>
 </file>
@@ -714,7 +714,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="65">
+  <borders count="66">
     <border>
       <left/>
       <right/>
@@ -1517,6 +1517,17 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -1528,7 +1539,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="184">
+  <cellXfs count="193">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1949,6 +1960,48 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1973,15 +2026,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2006,37 +2050,31 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="38" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="51" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="11" fillId="3" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="11" fillId="0" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="11" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="11" fillId="3" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="51" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="12" fillId="0" borderId="65" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2358,7 +2396,7 @@
   <dimension ref="B1:V103"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15:R15"/>
+      <selection activeCell="T19" sqref="T19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2408,24 +2446,24 @@
       <c r="R1" s="2"/>
     </row>
     <row r="2" spans="2:21" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="183" t="s">
+      <c r="B2" s="154" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="183"/>
-      <c r="D2" s="183"/>
-      <c r="E2" s="183"/>
-      <c r="F2" s="183"/>
-      <c r="G2" s="183"/>
-      <c r="H2" s="183"/>
-      <c r="I2" s="183"/>
-      <c r="J2" s="183"/>
-      <c r="K2" s="183"/>
-      <c r="L2" s="183"/>
-      <c r="M2" s="183"/>
-      <c r="N2" s="183"/>
-      <c r="O2" s="183"/>
-      <c r="P2" s="183"/>
-      <c r="Q2" s="183"/>
+      <c r="C2" s="154"/>
+      <c r="D2" s="154"/>
+      <c r="E2" s="154"/>
+      <c r="F2" s="154"/>
+      <c r="G2" s="154"/>
+      <c r="H2" s="154"/>
+      <c r="I2" s="154"/>
+      <c r="J2" s="154"/>
+      <c r="K2" s="154"/>
+      <c r="L2" s="154"/>
+      <c r="M2" s="154"/>
+      <c r="N2" s="154"/>
+      <c r="O2" s="154"/>
+      <c r="P2" s="154"/>
+      <c r="Q2" s="154"/>
       <c r="R2" s="5" t="s">
         <v>2</v>
       </c>
@@ -2547,27 +2585,27 @@
     <row r="10" spans="2:21" s="11" customFormat="1" ht="72.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="16"/>
       <c r="C10" s="8"/>
-      <c r="D10" s="173" t="s">
+      <c r="D10" s="155" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="174"/>
-      <c r="F10" s="174"/>
-      <c r="G10" s="174"/>
-      <c r="H10" s="174"/>
-      <c r="I10" s="174"/>
-      <c r="J10" s="175"/>
+      <c r="E10" s="156"/>
+      <c r="F10" s="156"/>
+      <c r="G10" s="156"/>
+      <c r="H10" s="156"/>
+      <c r="I10" s="156"/>
+      <c r="J10" s="157"/>
       <c r="K10" s="17"/>
-      <c r="L10" s="176" t="s">
+      <c r="L10" s="158" t="s">
         <v>14</v>
       </c>
-      <c r="M10" s="177"/>
+      <c r="M10" s="159"/>
       <c r="N10" s="17"/>
-      <c r="O10" s="173" t="s">
+      <c r="O10" s="155" t="s">
         <v>13</v>
       </c>
-      <c r="P10" s="174"/>
-      <c r="Q10" s="174"/>
-      <c r="R10" s="175"/>
+      <c r="P10" s="156"/>
+      <c r="Q10" s="156"/>
+      <c r="R10" s="157"/>
     </row>
     <row r="11" spans="2:21" ht="90" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="18" t="s">
@@ -2576,61 +2614,61 @@
       <c r="C11" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="178" t="s">
+      <c r="D11" s="160" t="s">
         <v>17</v>
       </c>
-      <c r="E11" s="178" t="s">
+      <c r="E11" s="160" t="s">
         <v>18</v>
       </c>
-      <c r="F11" s="178" t="s">
+      <c r="F11" s="160" t="s">
         <v>19</v>
       </c>
-      <c r="G11" s="178" t="s">
+      <c r="G11" s="160" t="s">
         <v>20</v>
       </c>
-      <c r="H11" s="180" t="s">
+      <c r="H11" s="162" t="s">
         <v>21</v>
       </c>
-      <c r="I11" s="162"/>
-      <c r="J11" s="163" t="s">
+      <c r="I11" s="163"/>
+      <c r="J11" s="164" t="s">
         <v>22</v>
       </c>
       <c r="K11" s="20"/>
-      <c r="L11" s="181" t="s">
+      <c r="L11" s="166" t="s">
         <v>23</v>
       </c>
-      <c r="M11" s="159" t="s">
+      <c r="M11" s="173" t="s">
         <v>24</v>
       </c>
       <c r="N11" s="21"/>
-      <c r="O11" s="161" t="s">
+      <c r="O11" s="175" t="s">
         <v>25</v>
       </c>
-      <c r="P11" s="162"/>
-      <c r="Q11" s="163" t="s">
+      <c r="P11" s="163"/>
+      <c r="Q11" s="164" t="s">
         <v>26</v>
       </c>
-      <c r="R11" s="165" t="s">
+      <c r="R11" s="176" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="12" spans="2:21" s="30" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="22"/>
       <c r="C12" s="23"/>
-      <c r="D12" s="179"/>
-      <c r="E12" s="179"/>
-      <c r="F12" s="179"/>
-      <c r="G12" s="179"/>
+      <c r="D12" s="161"/>
+      <c r="E12" s="161"/>
+      <c r="F12" s="161"/>
+      <c r="G12" s="161"/>
       <c r="H12" s="24" t="s">
         <v>28</v>
       </c>
       <c r="I12" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="J12" s="164"/>
+      <c r="J12" s="165"/>
       <c r="K12" s="25"/>
-      <c r="L12" s="182"/>
-      <c r="M12" s="160"/>
+      <c r="L12" s="167"/>
+      <c r="M12" s="174"/>
       <c r="N12" s="26"/>
       <c r="O12" s="27" t="s">
         <v>30</v>
@@ -2638,8 +2676,8 @@
       <c r="P12" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="Q12" s="164"/>
-      <c r="R12" s="166"/>
+      <c r="Q12" s="165"/>
+      <c r="R12" s="177"/>
       <c r="S12" s="29"/>
       <c r="T12" s="29"/>
       <c r="U12" s="29"/>
@@ -2690,46 +2728,46 @@
       </c>
     </row>
     <row r="14" spans="2:21" s="11" customFormat="1" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="167" t="s">
+      <c r="B14" s="178" t="s">
         <v>45</v>
       </c>
-      <c r="C14" s="168"/>
-      <c r="D14" s="168"/>
-      <c r="E14" s="168"/>
-      <c r="F14" s="168"/>
-      <c r="G14" s="168"/>
-      <c r="H14" s="168"/>
-      <c r="I14" s="168"/>
-      <c r="J14" s="168"/>
-      <c r="K14" s="168"/>
-      <c r="L14" s="168"/>
-      <c r="M14" s="168"/>
-      <c r="N14" s="168"/>
-      <c r="O14" s="168"/>
-      <c r="P14" s="168"/>
-      <c r="Q14" s="168"/>
-      <c r="R14" s="169"/>
+      <c r="C14" s="179"/>
+      <c r="D14" s="179"/>
+      <c r="E14" s="179"/>
+      <c r="F14" s="179"/>
+      <c r="G14" s="179"/>
+      <c r="H14" s="179"/>
+      <c r="I14" s="179"/>
+      <c r="J14" s="179"/>
+      <c r="K14" s="179"/>
+      <c r="L14" s="179"/>
+      <c r="M14" s="179"/>
+      <c r="N14" s="179"/>
+      <c r="O14" s="179"/>
+      <c r="P14" s="179"/>
+      <c r="Q14" s="179"/>
+      <c r="R14" s="180"/>
     </row>
     <row r="15" spans="2:21" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="170" t="s">
+      <c r="B15" s="181" t="s">
         <v>46</v>
       </c>
-      <c r="C15" s="171"/>
-      <c r="D15" s="171"/>
-      <c r="E15" s="171"/>
-      <c r="F15" s="171"/>
-      <c r="G15" s="171"/>
-      <c r="H15" s="171"/>
-      <c r="I15" s="171"/>
-      <c r="J15" s="171"/>
-      <c r="K15" s="171"/>
-      <c r="L15" s="171"/>
-      <c r="M15" s="171"/>
-      <c r="N15" s="171"/>
-      <c r="O15" s="171"/>
-      <c r="P15" s="171"/>
-      <c r="Q15" s="171"/>
-      <c r="R15" s="172"/>
+      <c r="C15" s="182"/>
+      <c r="D15" s="182"/>
+      <c r="E15" s="182"/>
+      <c r="F15" s="182"/>
+      <c r="G15" s="182"/>
+      <c r="H15" s="182"/>
+      <c r="I15" s="182"/>
+      <c r="J15" s="182"/>
+      <c r="K15" s="182"/>
+      <c r="L15" s="182"/>
+      <c r="M15" s="182"/>
+      <c r="N15" s="182"/>
+      <c r="O15" s="182"/>
+      <c r="P15" s="182"/>
+      <c r="Q15" s="182"/>
+      <c r="R15" s="183"/>
       <c r="S15" s="8"/>
     </row>
     <row r="16" spans="2:21" ht="73.5" customHeight="1" x14ac:dyDescent="0.45">
@@ -2760,7 +2798,7 @@
     </row>
     <row r="17" spans="2:18" ht="66.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B17" s="150" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C17" s="43">
         <v>30</v>
@@ -2784,64 +2822,64 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:18" s="3" customFormat="1" ht="71.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:18" ht="66.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B18" s="150" t="s">
+        <v>136</v>
+      </c>
+      <c r="C18" s="192">
+        <v>30</v>
+      </c>
+      <c r="D18" s="45"/>
+      <c r="E18" s="45"/>
+      <c r="F18" s="45"/>
+      <c r="G18" s="45"/>
+      <c r="H18" s="45"/>
+      <c r="I18" s="45"/>
+      <c r="J18" s="45"/>
+      <c r="K18" s="83"/>
+      <c r="L18" s="45"/>
+      <c r="M18" s="45"/>
+      <c r="N18" s="83"/>
+      <c r="O18" s="45"/>
+      <c r="P18" s="66"/>
+      <c r="Q18" s="45"/>
+      <c r="R18" s="54">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:18" s="3" customFormat="1" ht="71.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B19" s="184" t="s">
         <v>93</v>
       </c>
-      <c r="C18" s="43">
+      <c r="C19" s="185">
         <v>30</v>
       </c>
-      <c r="D18" s="55"/>
-      <c r="E18" s="56"/>
-      <c r="F18" s="56"/>
-      <c r="G18" s="55"/>
-      <c r="H18" s="56"/>
-      <c r="I18" s="56"/>
-      <c r="J18" s="57"/>
-      <c r="K18" s="47"/>
-      <c r="L18" s="48"/>
-      <c r="M18" s="49"/>
-      <c r="N18" s="50"/>
-      <c r="O18" s="58"/>
-      <c r="P18" s="52"/>
-      <c r="Q18" s="59"/>
-      <c r="R18" s="54">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="2:18" s="3" customFormat="1" ht="69" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B19" s="150" t="s">
+      <c r="D19" s="55"/>
+      <c r="E19" s="56"/>
+      <c r="F19" s="56"/>
+      <c r="G19" s="55"/>
+      <c r="H19" s="56"/>
+      <c r="I19" s="56"/>
+      <c r="J19" s="57"/>
+      <c r="K19" s="186"/>
+      <c r="L19" s="187"/>
+      <c r="M19" s="188"/>
+      <c r="N19" s="189"/>
+      <c r="O19" s="58"/>
+      <c r="P19" s="190"/>
+      <c r="Q19" s="59"/>
+      <c r="R19" s="191">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:18" s="3" customFormat="1" ht="69" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B20" s="150" t="s">
         <v>95</v>
       </c>
-      <c r="C19" s="43">
+      <c r="C20" s="43">
         <v>30</v>
-      </c>
-      <c r="D19" s="44"/>
-      <c r="E19" s="45"/>
-      <c r="F19" s="45"/>
-      <c r="G19" s="44"/>
-      <c r="H19" s="45"/>
-      <c r="I19" s="45"/>
-      <c r="J19" s="46"/>
-      <c r="K19" s="47"/>
-      <c r="L19" s="48"/>
-      <c r="M19" s="49"/>
-      <c r="N19" s="50"/>
-      <c r="O19" s="51"/>
-      <c r="P19" s="52"/>
-      <c r="Q19" s="53"/>
-      <c r="R19" s="54">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="2:18" s="3" customFormat="1" ht="54.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B20" s="150" t="s">
-        <v>94</v>
-      </c>
-      <c r="C20" s="43">
-        <v>60</v>
       </c>
       <c r="D20" s="44"/>
       <c r="E20" s="45"/>
@@ -2862,12 +2900,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:18" s="3" customFormat="1" ht="57.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:18" s="3" customFormat="1" ht="54.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B21" s="150" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C21" s="43">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="D21" s="44"/>
       <c r="E21" s="45"/>
@@ -2888,35 +2926,35 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:18" s="3" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="2:18" s="3" customFormat="1" ht="57.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B22" s="150" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C22" s="43">
-        <v>60</v>
-      </c>
-      <c r="D22" s="60"/>
-      <c r="E22" s="61"/>
-      <c r="F22" s="61"/>
-      <c r="G22" s="60"/>
-      <c r="H22" s="61"/>
-      <c r="I22" s="61"/>
-      <c r="J22" s="62"/>
+        <v>30</v>
+      </c>
+      <c r="D22" s="44"/>
+      <c r="E22" s="45"/>
+      <c r="F22" s="45"/>
+      <c r="G22" s="44"/>
+      <c r="H22" s="45"/>
+      <c r="I22" s="45"/>
+      <c r="J22" s="46"/>
       <c r="K22" s="47"/>
       <c r="L22" s="48"/>
       <c r="M22" s="49"/>
       <c r="N22" s="50"/>
-      <c r="O22" s="63"/>
+      <c r="O22" s="51"/>
       <c r="P22" s="52"/>
-      <c r="Q22" s="64"/>
+      <c r="Q22" s="53"/>
       <c r="R22" s="54">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:18" s="3" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="2:18" s="3" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B23" s="150" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="C23" s="43">
         <v>60</v>
@@ -2940,35 +2978,35 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:18" s="3" customFormat="1" ht="59.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="2:18" s="3" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B24" s="150" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="C24" s="43">
-        <v>30</v>
-      </c>
-      <c r="D24" s="44"/>
-      <c r="E24" s="45"/>
-      <c r="F24" s="45"/>
-      <c r="G24" s="44"/>
-      <c r="H24" s="45"/>
-      <c r="I24" s="45"/>
-      <c r="J24" s="46"/>
+        <v>60</v>
+      </c>
+      <c r="D24" s="60"/>
+      <c r="E24" s="61"/>
+      <c r="F24" s="61"/>
+      <c r="G24" s="60"/>
+      <c r="H24" s="61"/>
+      <c r="I24" s="61"/>
+      <c r="J24" s="62"/>
       <c r="K24" s="47"/>
       <c r="L24" s="48"/>
       <c r="M24" s="49"/>
       <c r="N24" s="50"/>
-      <c r="O24" s="51"/>
+      <c r="O24" s="63"/>
       <c r="P24" s="52"/>
-      <c r="Q24" s="53"/>
+      <c r="Q24" s="64"/>
       <c r="R24" s="54">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:18" s="3" customFormat="1" ht="57.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="2:18" s="3" customFormat="1" ht="59.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B25" s="150" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C25" s="43">
         <v>30</v>
@@ -2992,9 +3030,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:18" s="3" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="26" spans="2:18" s="3" customFormat="1" ht="57.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B26" s="150" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="C26" s="43">
         <v>30</v>
@@ -3150,7 +3188,7 @@
     </row>
     <row r="32" spans="2:18" ht="64.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B32" s="150" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C32" s="43">
         <v>60</v>
@@ -3176,7 +3214,7 @@
     </row>
     <row r="33" spans="2:22" ht="69.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B33" s="150" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C33" s="43">
         <v>60</v>
@@ -3202,7 +3240,7 @@
     </row>
     <row r="34" spans="2:22" ht="64.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B34" s="150" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C34" s="43">
         <v>60</v>
@@ -3276,7 +3314,7 @@
     </row>
     <row r="37" spans="2:22" ht="52.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B37" s="150" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C37" s="43">
         <v>60</v>
@@ -3302,7 +3340,7 @@
     </row>
     <row r="38" spans="2:22" ht="54" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B38" s="150" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C38" s="43">
         <v>60</v>
@@ -3328,7 +3366,7 @@
     </row>
     <row r="39" spans="2:22" ht="60" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B39" s="150" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C39" s="43">
         <v>60</v>
@@ -3357,7 +3395,7 @@
     </row>
     <row r="40" spans="2:22" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B40" s="150" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C40" s="43">
         <v>60</v>
@@ -3383,7 +3421,7 @@
     </row>
     <row r="41" spans="2:22" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B41" s="150" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C41" s="43">
         <v>90</v>
@@ -3409,7 +3447,7 @@
     </row>
     <row r="42" spans="2:22" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B42" s="152" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C42" s="77" t="s">
         <v>48</v>
@@ -3435,7 +3473,7 @@
     </row>
     <row r="43" spans="2:22" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B43" s="152" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C43" s="77" t="s">
         <v>48</v>
@@ -3487,7 +3525,7 @@
     </row>
     <row r="45" spans="2:22" s="3" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B45" s="150" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C45" s="77" t="s">
         <v>50</v>
@@ -3513,7 +3551,7 @@
     </row>
     <row r="46" spans="2:22" s="3" customFormat="1" ht="66.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B46" s="150" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C46" s="77" t="s">
         <v>51</v>
@@ -3565,7 +3603,7 @@
     </row>
     <row r="48" spans="2:22" s="11" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B48" s="151" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C48" s="78">
         <v>240</v>
@@ -3591,7 +3629,7 @@
     </row>
     <row r="49" spans="2:18" s="3" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B49" s="150" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C49" s="78">
         <v>480</v>
@@ -3617,7 +3655,7 @@
     </row>
     <row r="50" spans="2:18" s="3" customFormat="1" ht="73.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B50" s="150" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C50" s="77" t="s">
         <v>53</v>
@@ -3643,7 +3681,7 @@
     </row>
     <row r="51" spans="2:18" s="3" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B51" s="150" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C51" s="77">
         <v>60</v>
@@ -3669,7 +3707,7 @@
     </row>
     <row r="52" spans="2:18" s="3" customFormat="1" ht="59.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B52" s="150" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C52" s="77">
         <v>60</v>
@@ -3695,7 +3733,7 @@
     </row>
     <row r="53" spans="2:18" s="3" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B53" s="150" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C53" s="77">
         <v>60</v>
@@ -3721,7 +3759,7 @@
     </row>
     <row r="54" spans="2:18" s="3" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B54" s="150" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C54" s="77">
         <v>60</v>
@@ -3747,7 +3785,7 @@
     </row>
     <row r="55" spans="2:18" s="3" customFormat="1" ht="72" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B55" s="150" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C55" s="77" t="s">
         <v>55</v>
@@ -3794,7 +3832,7 @@
     </row>
     <row r="57" spans="2:18" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B57" s="150" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C57" s="43">
         <v>100</v>
@@ -3820,7 +3858,7 @@
     </row>
     <row r="58" spans="2:18" ht="59.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B58" s="150" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C58" s="81" t="s">
         <v>51</v>
@@ -3846,7 +3884,7 @@
     </row>
     <row r="59" spans="2:18" ht="55.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B59" s="150" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C59" s="43">
         <v>100</v>
@@ -3872,7 +3910,7 @@
     </row>
     <row r="60" spans="2:18" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B60" s="150" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C60" s="82">
         <v>100</v>
@@ -3898,7 +3936,7 @@
     </row>
     <row r="61" spans="2:18" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B61" s="150" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C61" s="82">
         <v>100</v>
@@ -3950,7 +3988,7 @@
     </row>
     <row r="63" spans="2:18" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B63" s="150" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C63" s="43">
         <v>30</v>
@@ -4002,7 +4040,7 @@
     </row>
     <row r="65" spans="2:18" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B65" s="150" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C65" s="43">
         <v>100</v>
@@ -4028,7 +4066,7 @@
     </row>
     <row r="66" spans="2:18" ht="50.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B66" s="150" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C66" s="82">
         <v>100</v>
@@ -4054,7 +4092,7 @@
     </row>
     <row r="67" spans="2:18" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B67" s="153" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C67" s="85">
         <v>100</v>
@@ -4105,25 +4143,25 @@
       </c>
     </row>
     <row r="69" spans="2:18" s="86" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B69" s="154" t="s">
+      <c r="B69" s="168" t="s">
         <v>61</v>
       </c>
-      <c r="C69" s="154"/>
-      <c r="D69" s="154"/>
-      <c r="E69" s="154"/>
-      <c r="F69" s="154"/>
-      <c r="G69" s="154"/>
-      <c r="H69" s="154"/>
-      <c r="I69" s="154"/>
-      <c r="J69" s="154"/>
-      <c r="K69" s="154"/>
-      <c r="L69" s="154"/>
-      <c r="M69" s="154"/>
-      <c r="N69" s="155"/>
-      <c r="O69" s="154"/>
-      <c r="P69" s="154"/>
-      <c r="Q69" s="154"/>
-      <c r="R69" s="154"/>
+      <c r="C69" s="168"/>
+      <c r="D69" s="168"/>
+      <c r="E69" s="168"/>
+      <c r="F69" s="168"/>
+      <c r="G69" s="168"/>
+      <c r="H69" s="168"/>
+      <c r="I69" s="168"/>
+      <c r="J69" s="168"/>
+      <c r="K69" s="168"/>
+      <c r="L69" s="168"/>
+      <c r="M69" s="168"/>
+      <c r="N69" s="169"/>
+      <c r="O69" s="168"/>
+      <c r="P69" s="168"/>
+      <c r="Q69" s="168"/>
+      <c r="R69" s="168"/>
     </row>
     <row r="70" spans="2:18" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B70" s="153" t="s">
@@ -4234,61 +4272,61 @@
       <c r="R75" s="92"/>
     </row>
     <row r="76" spans="2:18" s="93" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B76" s="156"/>
-      <c r="C76" s="156"/>
-      <c r="D76" s="156"/>
-      <c r="E76" s="156"/>
-      <c r="F76" s="156"/>
-      <c r="G76" s="156"/>
-      <c r="H76" s="156"/>
-      <c r="I76" s="156"/>
-      <c r="J76" s="156"/>
-      <c r="K76" s="156"/>
-      <c r="L76" s="156"/>
-      <c r="M76" s="156"/>
-      <c r="N76" s="156"/>
-      <c r="O76" s="156"/>
-      <c r="P76" s="156"/>
-      <c r="Q76" s="156"/>
-      <c r="R76" s="156"/>
+      <c r="B76" s="170"/>
+      <c r="C76" s="170"/>
+      <c r="D76" s="170"/>
+      <c r="E76" s="170"/>
+      <c r="F76" s="170"/>
+      <c r="G76" s="170"/>
+      <c r="H76" s="170"/>
+      <c r="I76" s="170"/>
+      <c r="J76" s="170"/>
+      <c r="K76" s="170"/>
+      <c r="L76" s="170"/>
+      <c r="M76" s="170"/>
+      <c r="N76" s="170"/>
+      <c r="O76" s="170"/>
+      <c r="P76" s="170"/>
+      <c r="Q76" s="170"/>
+      <c r="R76" s="170"/>
     </row>
     <row r="77" spans="2:18" s="93" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B77" s="157"/>
-      <c r="C77" s="157"/>
-      <c r="D77" s="157"/>
-      <c r="E77" s="157"/>
-      <c r="F77" s="157"/>
-      <c r="G77" s="157"/>
-      <c r="H77" s="157"/>
-      <c r="I77" s="157"/>
-      <c r="J77" s="157"/>
-      <c r="K77" s="157"/>
-      <c r="L77" s="157"/>
-      <c r="M77" s="157"/>
-      <c r="N77" s="157"/>
-      <c r="O77" s="157"/>
-      <c r="P77" s="157"/>
-      <c r="Q77" s="157"/>
-      <c r="R77" s="157"/>
+      <c r="B77" s="171"/>
+      <c r="C77" s="171"/>
+      <c r="D77" s="171"/>
+      <c r="E77" s="171"/>
+      <c r="F77" s="171"/>
+      <c r="G77" s="171"/>
+      <c r="H77" s="171"/>
+      <c r="I77" s="171"/>
+      <c r="J77" s="171"/>
+      <c r="K77" s="171"/>
+      <c r="L77" s="171"/>
+      <c r="M77" s="171"/>
+      <c r="N77" s="171"/>
+      <c r="O77" s="171"/>
+      <c r="P77" s="171"/>
+      <c r="Q77" s="171"/>
+      <c r="R77" s="171"/>
     </row>
     <row r="78" spans="2:18" s="93" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B78" s="158"/>
-      <c r="C78" s="158"/>
-      <c r="D78" s="158"/>
-      <c r="E78" s="158"/>
-      <c r="F78" s="158"/>
-      <c r="G78" s="158"/>
-      <c r="H78" s="158"/>
-      <c r="I78" s="158"/>
-      <c r="J78" s="158"/>
-      <c r="K78" s="158"/>
-      <c r="L78" s="158"/>
-      <c r="M78" s="158"/>
-      <c r="N78" s="158"/>
-      <c r="O78" s="158"/>
-      <c r="P78" s="158"/>
-      <c r="Q78" s="158"/>
-      <c r="R78" s="158"/>
+      <c r="B78" s="172"/>
+      <c r="C78" s="172"/>
+      <c r="D78" s="172"/>
+      <c r="E78" s="172"/>
+      <c r="F78" s="172"/>
+      <c r="G78" s="172"/>
+      <c r="H78" s="172"/>
+      <c r="I78" s="172"/>
+      <c r="J78" s="172"/>
+      <c r="K78" s="172"/>
+      <c r="L78" s="172"/>
+      <c r="M78" s="172"/>
+      <c r="N78" s="172"/>
+      <c r="O78" s="172"/>
+      <c r="P78" s="172"/>
+      <c r="Q78" s="172"/>
+      <c r="R78" s="172"/>
     </row>
     <row r="79" spans="2:18" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="B79" s="94"/>
@@ -4732,6 +4770,15 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B69:N69"/>
+    <mergeCell ref="O69:R69"/>
+    <mergeCell ref="B76:R78"/>
+    <mergeCell ref="M11:M12"/>
+    <mergeCell ref="O11:P11"/>
+    <mergeCell ref="Q11:Q12"/>
+    <mergeCell ref="R11:R12"/>
+    <mergeCell ref="B14:R14"/>
+    <mergeCell ref="B15:R15"/>
     <mergeCell ref="B2:Q2"/>
     <mergeCell ref="D10:J10"/>
     <mergeCell ref="L10:M10"/>
@@ -4743,15 +4790,6 @@
     <mergeCell ref="H11:I11"/>
     <mergeCell ref="J11:J12"/>
     <mergeCell ref="L11:L12"/>
-    <mergeCell ref="B69:N69"/>
-    <mergeCell ref="O69:R69"/>
-    <mergeCell ref="B76:R78"/>
-    <mergeCell ref="M11:M12"/>
-    <mergeCell ref="O11:P11"/>
-    <mergeCell ref="Q11:Q12"/>
-    <mergeCell ref="R11:R12"/>
-    <mergeCell ref="B14:R14"/>
-    <mergeCell ref="B15:R15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
#Fixed: Modified packsize in cdrr templates
</commit_message>
<xml_diff>
--- a/assets/templates/orders/v2/cdrr_aggregate.xlsx
+++ b/assets/templates/orders/v2/cdrr_aggregate.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18528"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -1960,6 +1960,90 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="51" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="11" fillId="3" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="11" fillId="0" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="11" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="11" fillId="3" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="51" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="12" fillId="0" borderId="65" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="38" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="58" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="38" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1987,95 +2071,11 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="38" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="58" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="38" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="51" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="11" fillId="3" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="11" fillId="0" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="11" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="11" fillId="3" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="51" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="12" fillId="0" borderId="65" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2395,8 +2395,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:V103"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="T19" sqref="T19"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2446,24 +2446,24 @@
       <c r="R1" s="2"/>
     </row>
     <row r="2" spans="2:21" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="154" t="s">
+      <c r="B2" s="182" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="154"/>
-      <c r="D2" s="154"/>
-      <c r="E2" s="154"/>
-      <c r="F2" s="154"/>
-      <c r="G2" s="154"/>
-      <c r="H2" s="154"/>
-      <c r="I2" s="154"/>
-      <c r="J2" s="154"/>
-      <c r="K2" s="154"/>
-      <c r="L2" s="154"/>
-      <c r="M2" s="154"/>
-      <c r="N2" s="154"/>
-      <c r="O2" s="154"/>
-      <c r="P2" s="154"/>
-      <c r="Q2" s="154"/>
+      <c r="C2" s="182"/>
+      <c r="D2" s="182"/>
+      <c r="E2" s="182"/>
+      <c r="F2" s="182"/>
+      <c r="G2" s="182"/>
+      <c r="H2" s="182"/>
+      <c r="I2" s="182"/>
+      <c r="J2" s="182"/>
+      <c r="K2" s="182"/>
+      <c r="L2" s="182"/>
+      <c r="M2" s="182"/>
+      <c r="N2" s="182"/>
+      <c r="O2" s="182"/>
+      <c r="P2" s="182"/>
+      <c r="Q2" s="182"/>
       <c r="R2" s="5" t="s">
         <v>2</v>
       </c>
@@ -2585,27 +2585,27 @@
     <row r="10" spans="2:21" s="11" customFormat="1" ht="72.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="16"/>
       <c r="C10" s="8"/>
-      <c r="D10" s="155" t="s">
+      <c r="D10" s="183" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="156"/>
-      <c r="F10" s="156"/>
-      <c r="G10" s="156"/>
-      <c r="H10" s="156"/>
-      <c r="I10" s="156"/>
-      <c r="J10" s="157"/>
+      <c r="E10" s="184"/>
+      <c r="F10" s="184"/>
+      <c r="G10" s="184"/>
+      <c r="H10" s="184"/>
+      <c r="I10" s="184"/>
+      <c r="J10" s="185"/>
       <c r="K10" s="17"/>
-      <c r="L10" s="158" t="s">
+      <c r="L10" s="186" t="s">
         <v>14</v>
       </c>
-      <c r="M10" s="159"/>
+      <c r="M10" s="187"/>
       <c r="N10" s="17"/>
-      <c r="O10" s="155" t="s">
+      <c r="O10" s="183" t="s">
         <v>13</v>
       </c>
-      <c r="P10" s="156"/>
-      <c r="Q10" s="156"/>
-      <c r="R10" s="157"/>
+      <c r="P10" s="184"/>
+      <c r="Q10" s="184"/>
+      <c r="R10" s="185"/>
     </row>
     <row r="11" spans="2:21" ht="90" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="18" t="s">
@@ -2614,61 +2614,61 @@
       <c r="C11" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="160" t="s">
+      <c r="D11" s="188" t="s">
         <v>17</v>
       </c>
-      <c r="E11" s="160" t="s">
+      <c r="E11" s="188" t="s">
         <v>18</v>
       </c>
-      <c r="F11" s="160" t="s">
+      <c r="F11" s="188" t="s">
         <v>19</v>
       </c>
-      <c r="G11" s="160" t="s">
+      <c r="G11" s="188" t="s">
         <v>20</v>
       </c>
-      <c r="H11" s="162" t="s">
+      <c r="H11" s="190" t="s">
         <v>21</v>
       </c>
-      <c r="I11" s="163"/>
-      <c r="J11" s="164" t="s">
+      <c r="I11" s="171"/>
+      <c r="J11" s="172" t="s">
         <v>22</v>
       </c>
       <c r="K11" s="20"/>
-      <c r="L11" s="166" t="s">
+      <c r="L11" s="191" t="s">
         <v>23</v>
       </c>
-      <c r="M11" s="173" t="s">
+      <c r="M11" s="168" t="s">
         <v>24</v>
       </c>
       <c r="N11" s="21"/>
-      <c r="O11" s="175" t="s">
+      <c r="O11" s="170" t="s">
         <v>25</v>
       </c>
-      <c r="P11" s="163"/>
-      <c r="Q11" s="164" t="s">
+      <c r="P11" s="171"/>
+      <c r="Q11" s="172" t="s">
         <v>26</v>
       </c>
-      <c r="R11" s="176" t="s">
+      <c r="R11" s="174" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="12" spans="2:21" s="30" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="22"/>
       <c r="C12" s="23"/>
-      <c r="D12" s="161"/>
-      <c r="E12" s="161"/>
-      <c r="F12" s="161"/>
-      <c r="G12" s="161"/>
+      <c r="D12" s="189"/>
+      <c r="E12" s="189"/>
+      <c r="F12" s="189"/>
+      <c r="G12" s="189"/>
       <c r="H12" s="24" t="s">
         <v>28</v>
       </c>
       <c r="I12" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="J12" s="165"/>
+      <c r="J12" s="173"/>
       <c r="K12" s="25"/>
-      <c r="L12" s="167"/>
-      <c r="M12" s="174"/>
+      <c r="L12" s="192"/>
+      <c r="M12" s="169"/>
       <c r="N12" s="26"/>
       <c r="O12" s="27" t="s">
         <v>30</v>
@@ -2676,8 +2676,8 @@
       <c r="P12" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="Q12" s="165"/>
-      <c r="R12" s="177"/>
+      <c r="Q12" s="173"/>
+      <c r="R12" s="175"/>
       <c r="S12" s="29"/>
       <c r="T12" s="29"/>
       <c r="U12" s="29"/>
@@ -2728,46 +2728,46 @@
       </c>
     </row>
     <row r="14" spans="2:21" s="11" customFormat="1" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="178" t="s">
+      <c r="B14" s="176" t="s">
         <v>45</v>
       </c>
-      <c r="C14" s="179"/>
-      <c r="D14" s="179"/>
-      <c r="E14" s="179"/>
-      <c r="F14" s="179"/>
-      <c r="G14" s="179"/>
-      <c r="H14" s="179"/>
-      <c r="I14" s="179"/>
-      <c r="J14" s="179"/>
-      <c r="K14" s="179"/>
-      <c r="L14" s="179"/>
-      <c r="M14" s="179"/>
-      <c r="N14" s="179"/>
-      <c r="O14" s="179"/>
-      <c r="P14" s="179"/>
-      <c r="Q14" s="179"/>
-      <c r="R14" s="180"/>
+      <c r="C14" s="177"/>
+      <c r="D14" s="177"/>
+      <c r="E14" s="177"/>
+      <c r="F14" s="177"/>
+      <c r="G14" s="177"/>
+      <c r="H14" s="177"/>
+      <c r="I14" s="177"/>
+      <c r="J14" s="177"/>
+      <c r="K14" s="177"/>
+      <c r="L14" s="177"/>
+      <c r="M14" s="177"/>
+      <c r="N14" s="177"/>
+      <c r="O14" s="177"/>
+      <c r="P14" s="177"/>
+      <c r="Q14" s="177"/>
+      <c r="R14" s="178"/>
     </row>
     <row r="15" spans="2:21" s="11" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="181" t="s">
+      <c r="B15" s="179" t="s">
         <v>46</v>
       </c>
-      <c r="C15" s="182"/>
-      <c r="D15" s="182"/>
-      <c r="E15" s="182"/>
-      <c r="F15" s="182"/>
-      <c r="G15" s="182"/>
-      <c r="H15" s="182"/>
-      <c r="I15" s="182"/>
-      <c r="J15" s="182"/>
-      <c r="K15" s="182"/>
-      <c r="L15" s="182"/>
-      <c r="M15" s="182"/>
-      <c r="N15" s="182"/>
-      <c r="O15" s="182"/>
-      <c r="P15" s="182"/>
-      <c r="Q15" s="182"/>
-      <c r="R15" s="183"/>
+      <c r="C15" s="180"/>
+      <c r="D15" s="180"/>
+      <c r="E15" s="180"/>
+      <c r="F15" s="180"/>
+      <c r="G15" s="180"/>
+      <c r="H15" s="180"/>
+      <c r="I15" s="180"/>
+      <c r="J15" s="180"/>
+      <c r="K15" s="180"/>
+      <c r="L15" s="180"/>
+      <c r="M15" s="180"/>
+      <c r="N15" s="180"/>
+      <c r="O15" s="180"/>
+      <c r="P15" s="180"/>
+      <c r="Q15" s="180"/>
+      <c r="R15" s="181"/>
       <c r="S15" s="8"/>
     </row>
     <row r="16" spans="2:21" ht="73.5" customHeight="1" x14ac:dyDescent="0.45">
@@ -2826,7 +2826,7 @@
       <c r="B18" s="150" t="s">
         <v>136</v>
       </c>
-      <c r="C18" s="192">
+      <c r="C18" s="162">
         <v>30</v>
       </c>
       <c r="D18" s="45"/>
@@ -2849,10 +2849,10 @@
       </c>
     </row>
     <row r="19" spans="2:18" s="3" customFormat="1" ht="71.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B19" s="184" t="s">
+      <c r="B19" s="154" t="s">
         <v>93</v>
       </c>
-      <c r="C19" s="185">
+      <c r="C19" s="155">
         <v>30</v>
       </c>
       <c r="D19" s="55"/>
@@ -2862,14 +2862,14 @@
       <c r="H19" s="56"/>
       <c r="I19" s="56"/>
       <c r="J19" s="57"/>
-      <c r="K19" s="186"/>
-      <c r="L19" s="187"/>
-      <c r="M19" s="188"/>
-      <c r="N19" s="189"/>
+      <c r="K19" s="156"/>
+      <c r="L19" s="157"/>
+      <c r="M19" s="158"/>
+      <c r="N19" s="159"/>
       <c r="O19" s="58"/>
-      <c r="P19" s="190"/>
+      <c r="P19" s="160"/>
       <c r="Q19" s="59"/>
-      <c r="R19" s="191">
+      <c r="R19" s="161">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2931,7 +2931,7 @@
         <v>96</v>
       </c>
       <c r="C22" s="43">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="D22" s="44"/>
       <c r="E22" s="45"/>
@@ -4143,25 +4143,25 @@
       </c>
     </row>
     <row r="69" spans="2:18" s="86" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B69" s="168" t="s">
+      <c r="B69" s="163" t="s">
         <v>61</v>
       </c>
-      <c r="C69" s="168"/>
-      <c r="D69" s="168"/>
-      <c r="E69" s="168"/>
-      <c r="F69" s="168"/>
-      <c r="G69" s="168"/>
-      <c r="H69" s="168"/>
-      <c r="I69" s="168"/>
-      <c r="J69" s="168"/>
-      <c r="K69" s="168"/>
-      <c r="L69" s="168"/>
-      <c r="M69" s="168"/>
-      <c r="N69" s="169"/>
-      <c r="O69" s="168"/>
-      <c r="P69" s="168"/>
-      <c r="Q69" s="168"/>
-      <c r="R69" s="168"/>
+      <c r="C69" s="163"/>
+      <c r="D69" s="163"/>
+      <c r="E69" s="163"/>
+      <c r="F69" s="163"/>
+      <c r="G69" s="163"/>
+      <c r="H69" s="163"/>
+      <c r="I69" s="163"/>
+      <c r="J69" s="163"/>
+      <c r="K69" s="163"/>
+      <c r="L69" s="163"/>
+      <c r="M69" s="163"/>
+      <c r="N69" s="164"/>
+      <c r="O69" s="163"/>
+      <c r="P69" s="163"/>
+      <c r="Q69" s="163"/>
+      <c r="R69" s="163"/>
     </row>
     <row r="70" spans="2:18" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B70" s="153" t="s">
@@ -4272,61 +4272,61 @@
       <c r="R75" s="92"/>
     </row>
     <row r="76" spans="2:18" s="93" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B76" s="170"/>
-      <c r="C76" s="170"/>
-      <c r="D76" s="170"/>
-      <c r="E76" s="170"/>
-      <c r="F76" s="170"/>
-      <c r="G76" s="170"/>
-      <c r="H76" s="170"/>
-      <c r="I76" s="170"/>
-      <c r="J76" s="170"/>
-      <c r="K76" s="170"/>
-      <c r="L76" s="170"/>
-      <c r="M76" s="170"/>
-      <c r="N76" s="170"/>
-      <c r="O76" s="170"/>
-      <c r="P76" s="170"/>
-      <c r="Q76" s="170"/>
-      <c r="R76" s="170"/>
+      <c r="B76" s="165"/>
+      <c r="C76" s="165"/>
+      <c r="D76" s="165"/>
+      <c r="E76" s="165"/>
+      <c r="F76" s="165"/>
+      <c r="G76" s="165"/>
+      <c r="H76" s="165"/>
+      <c r="I76" s="165"/>
+      <c r="J76" s="165"/>
+      <c r="K76" s="165"/>
+      <c r="L76" s="165"/>
+      <c r="M76" s="165"/>
+      <c r="N76" s="165"/>
+      <c r="O76" s="165"/>
+      <c r="P76" s="165"/>
+      <c r="Q76" s="165"/>
+      <c r="R76" s="165"/>
     </row>
     <row r="77" spans="2:18" s="93" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B77" s="171"/>
-      <c r="C77" s="171"/>
-      <c r="D77" s="171"/>
-      <c r="E77" s="171"/>
-      <c r="F77" s="171"/>
-      <c r="G77" s="171"/>
-      <c r="H77" s="171"/>
-      <c r="I77" s="171"/>
-      <c r="J77" s="171"/>
-      <c r="K77" s="171"/>
-      <c r="L77" s="171"/>
-      <c r="M77" s="171"/>
-      <c r="N77" s="171"/>
-      <c r="O77" s="171"/>
-      <c r="P77" s="171"/>
-      <c r="Q77" s="171"/>
-      <c r="R77" s="171"/>
+      <c r="B77" s="166"/>
+      <c r="C77" s="166"/>
+      <c r="D77" s="166"/>
+      <c r="E77" s="166"/>
+      <c r="F77" s="166"/>
+      <c r="G77" s="166"/>
+      <c r="H77" s="166"/>
+      <c r="I77" s="166"/>
+      <c r="J77" s="166"/>
+      <c r="K77" s="166"/>
+      <c r="L77" s="166"/>
+      <c r="M77" s="166"/>
+      <c r="N77" s="166"/>
+      <c r="O77" s="166"/>
+      <c r="P77" s="166"/>
+      <c r="Q77" s="166"/>
+      <c r="R77" s="166"/>
     </row>
     <row r="78" spans="2:18" s="93" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B78" s="172"/>
-      <c r="C78" s="172"/>
-      <c r="D78" s="172"/>
-      <c r="E78" s="172"/>
-      <c r="F78" s="172"/>
-      <c r="G78" s="172"/>
-      <c r="H78" s="172"/>
-      <c r="I78" s="172"/>
-      <c r="J78" s="172"/>
-      <c r="K78" s="172"/>
-      <c r="L78" s="172"/>
-      <c r="M78" s="172"/>
-      <c r="N78" s="172"/>
-      <c r="O78" s="172"/>
-      <c r="P78" s="172"/>
-      <c r="Q78" s="172"/>
-      <c r="R78" s="172"/>
+      <c r="B78" s="167"/>
+      <c r="C78" s="167"/>
+      <c r="D78" s="167"/>
+      <c r="E78" s="167"/>
+      <c r="F78" s="167"/>
+      <c r="G78" s="167"/>
+      <c r="H78" s="167"/>
+      <c r="I78" s="167"/>
+      <c r="J78" s="167"/>
+      <c r="K78" s="167"/>
+      <c r="L78" s="167"/>
+      <c r="M78" s="167"/>
+      <c r="N78" s="167"/>
+      <c r="O78" s="167"/>
+      <c r="P78" s="167"/>
+      <c r="Q78" s="167"/>
+      <c r="R78" s="167"/>
     </row>
     <row r="79" spans="2:18" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="B79" s="94"/>
@@ -4770,15 +4770,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="B69:N69"/>
-    <mergeCell ref="O69:R69"/>
-    <mergeCell ref="B76:R78"/>
-    <mergeCell ref="M11:M12"/>
-    <mergeCell ref="O11:P11"/>
-    <mergeCell ref="Q11:Q12"/>
-    <mergeCell ref="R11:R12"/>
-    <mergeCell ref="B14:R14"/>
-    <mergeCell ref="B15:R15"/>
     <mergeCell ref="B2:Q2"/>
     <mergeCell ref="D10:J10"/>
     <mergeCell ref="L10:M10"/>
@@ -4790,6 +4781,15 @@
     <mergeCell ref="H11:I11"/>
     <mergeCell ref="J11:J12"/>
     <mergeCell ref="L11:L12"/>
+    <mergeCell ref="B69:N69"/>
+    <mergeCell ref="O69:R69"/>
+    <mergeCell ref="B76:R78"/>
+    <mergeCell ref="M11:M12"/>
+    <mergeCell ref="O11:P11"/>
+    <mergeCell ref="Q11:Q12"/>
+    <mergeCell ref="R11:R12"/>
+    <mergeCell ref="B14:R14"/>
+    <mergeCell ref="B15:R15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>